<commit_message>
Se puede agregar muestras desde un excel
</commit_message>
<xml_diff>
--- a/src/excel/muestras.xlsx
+++ b/src/excel/muestras.xlsx
@@ -11,25 +11,40 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Carga de Muestras</t>
   </si>
   <si>
-    <t>Muestra excel de ejemplo</t>
+    <t>Numero de orden</t>
+  </si>
+  <si>
+    <t>Titulo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">responsable (via mail) </t>
+  </si>
+  <si>
+    <t>Horas aprox</t>
+  </si>
+  <si>
+    <t>Notas</t>
+  </si>
+  <si>
+    <t>Muestra desde excel</t>
   </si>
   <si>
     <t>alicemarcelaramirez@gmail.com</t>
   </si>
   <si>
-    <t>Notas de excel.</t>
+    <t>Notas desde excel...</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -42,9 +57,19 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF0563C1"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <u/>
@@ -53,12 +78,18 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4A86E8"/>
+        <bgColor rgb="FF4A86E8"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -67,17 +98,21 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -294,11 +329,11 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="16.86"/>
-    <col customWidth="1" min="2" max="2" width="27.29"/>
-    <col customWidth="1" min="3" max="3" width="21.29"/>
+    <col customWidth="1" min="1" max="1" width="21.29"/>
+    <col customWidth="1" min="2" max="2" width="25.43"/>
+    <col customWidth="1" min="3" max="3" width="27.57"/>
     <col customWidth="1" min="4" max="4" width="11.43"/>
-    <col customWidth="1" min="5" max="5" width="24.43"/>
+    <col customWidth="1" min="5" max="5" width="29.0"/>
     <col customWidth="1" min="6" max="26" width="9.14"/>
   </cols>
   <sheetData>
@@ -308,60 +343,74 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2">
-        <v>3.0</v>
+      <c r="A2" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
-      <c r="D2" s="2">
-        <v>4.0</v>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">
-      <c r="C3" s="3"/>
+      <c r="A3" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="3">
+        <v>5.0</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="4">
-      <c r="C4" s="3"/>
+      <c r="C4" s="5"/>
     </row>
     <row r="5">
-      <c r="C5" s="3"/>
+      <c r="C5" s="5"/>
     </row>
     <row r="6">
-      <c r="C6" s="3"/>
+      <c r="C6" s="5"/>
     </row>
     <row r="7">
-      <c r="C7" s="3"/>
+      <c r="C7" s="5"/>
     </row>
     <row r="8">
-      <c r="C8" s="3"/>
+      <c r="C8" s="5"/>
     </row>
     <row r="9">
-      <c r="C9" s="3"/>
+      <c r="C9" s="5"/>
     </row>
     <row r="10">
-      <c r="C10" s="3"/>
+      <c r="C10" s="5"/>
     </row>
     <row r="11">
-      <c r="C11" s="3"/>
+      <c r="C11" s="5"/>
     </row>
     <row r="12">
-      <c r="C12" s="3"/>
+      <c r="C12" s="5"/>
     </row>
     <row r="13">
-      <c r="C13" s="3"/>
+      <c r="C13" s="5"/>
     </row>
     <row r="14">
-      <c r="C14" s="3"/>
+      <c r="C14" s="5"/>
     </row>
     <row r="15">
-      <c r="C15" s="3"/>
+      <c r="C15" s="5"/>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>

</xml_diff>